<commit_message>
add stfips to output
</commit_message>
<xml_diff>
--- a/Population/PopPyramid2016.xlsx
+++ b/Population/PopPyramid2016.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
   <si>
     <t>2016 Total Population</t>
   </si>
@@ -23,6 +23,12 @@
   </si>
   <si>
     <t>2016 Female</t>
+  </si>
+  <si>
+    <t>stfips</t>
+  </si>
+  <si>
+    <t>05</t>
   </si>
 </sst>
 </file>
@@ -380,13 +386,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,8 +402,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>744934</v>
       </c>
@@ -407,8 +416,11 @@
       <c r="C2">
         <v>363574</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>287610</v>
       </c>
@@ -418,8 +430,11 @@
       <c r="C3">
         <v>141093</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>388024</v>
       </c>
@@ -429,8 +444,11 @@
       <c r="C4">
         <v>193596</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>364093</v>
       </c>
@@ -440,8 +458,11 @@
       <c r="C5">
         <v>183479</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>380299</v>
       </c>
@@ -451,8 +472,11 @@
       <c r="C6">
         <v>192911</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>370732</v>
       </c>
@@ -462,8 +486,11 @@
       <c r="C7">
         <v>193038</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>270051</v>
       </c>
@@ -473,8 +500,11 @@
       <c r="C8">
         <v>144284</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>184175</v>
       </c>
@@ -484,8 +514,11 @@
       <c r="C9">
         <v>108990</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>2989918</v>
       </c>
@@ -494,6 +527,9 @@
       </c>
       <c r="C10">
         <v>1520965</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>